<commit_message>
Insersão de dados normal funcionando
</commit_message>
<xml_diff>
--- a/PLANILHA MÓDULOS V0.xlsx
+++ b/PLANILHA MÓDULOS V0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel Guido\Desktop\Github Repositories\PrimeiroBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42670BFE-4CB0-4B6E-8C6D-0B2287E10549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F7689AB-9579-4B3A-86B1-E13E280D8F06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="982" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60" yWindow="15" windowWidth="20460" windowHeight="10770" tabRatio="982" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exemplos Módulo" sheetId="11" r:id="rId1"/>
@@ -35,7 +35,7 @@
     <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="3">Dietas!$A$1:$A$129</definedName>
     <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0" localSheetId="3">Dietas!$A$1:$A$129</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3">Dietas!$A$1:$A$129</definedName>
-    <definedName name="a" localSheetId="0">'Exemplos Módulo'!$A$1:$S$28</definedName>
+    <definedName name="a" localSheetId="0">'Exemplos Módulo'!$A$1:$S$29</definedName>
     <definedName name="a" localSheetId="1">Pedidos!$A$1:$S$88</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="281">
   <si>
     <t>DOCUMENTO RETIDO
 PLANILHA DE PEDIDOS PADRONIZADOS</t>
@@ -740,9 +740,6 @@
     <t>Horários de Entrega</t>
   </si>
   <si>
-    <t>14:00</t>
-  </si>
-  <si>
     <t>Unidades de Internação</t>
   </si>
   <si>
@@ -888,6 +885,9 @@
   </si>
   <si>
     <t>PACIENTE 08</t>
+  </si>
+  <si>
+    <t>14:30</t>
   </si>
 </sst>
 </file>
@@ -1161,7 +1161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1410,6 +1410,9 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1428,6 +1431,27 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1436,27 +1460,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2073,12 +2076,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S875"/>
+  <dimension ref="A1:S876"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="8" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="U20" sqref="U20"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2104,68 +2107,68 @@
   <sheetData>
     <row r="1" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="84" t="s">
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
-      <c r="K1" s="84"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="85" t="s">
-        <v>270</v>
-      </c>
-      <c r="N1" s="85"/>
-      <c r="O1" s="85"/>
-      <c r="P1" s="85"/>
-      <c r="Q1" s="85"/>
-      <c r="R1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
+      <c r="L1" s="85"/>
+      <c r="M1" s="86" t="s">
+        <v>269</v>
+      </c>
+      <c r="N1" s="86"/>
+      <c r="O1" s="86"/>
+      <c r="P1" s="86"/>
+      <c r="Q1" s="86"/>
+      <c r="R1" s="86"/>
     </row>
     <row r="2" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="85"/>
-      <c r="N2" s="85"/>
-      <c r="O2" s="85"/>
-      <c r="P2" s="85"/>
-      <c r="Q2" s="85"/>
-      <c r="R2" s="85"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="86"/>
+      <c r="O2" s="86"/>
+      <c r="P2" s="86"/>
+      <c r="Q2" s="86"/>
+      <c r="R2" s="86"/>
       <c r="S2" s="4"/>
     </row>
     <row r="3" spans="1:19" ht="3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
-      <c r="B3" s="83"/>
-      <c r="C3" s="83"/>
-      <c r="D3" s="83"/>
-      <c r="E3" s="83"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="84"/>
-      <c r="H3" s="84"/>
-      <c r="I3" s="84"/>
-      <c r="J3" s="84"/>
-      <c r="K3" s="84"/>
-      <c r="L3" s="84"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="85"/>
-      <c r="O3" s="85"/>
-      <c r="P3" s="85"/>
-      <c r="Q3" s="85"/>
-      <c r="R3" s="85"/>
+      <c r="B3" s="84"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="86"/>
+      <c r="N3" s="86"/>
+      <c r="O3" s="86"/>
+      <c r="P3" s="86"/>
+      <c r="Q3" s="86"/>
+      <c r="R3" s="86"/>
       <c r="S3" s="4"/>
     </row>
     <row r="4" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2196,7 +2199,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H5" s="15"/>
       <c r="I5" s="13"/>
@@ -2205,7 +2208,7 @@
         <v>3</v>
       </c>
       <c r="L5" s="64" t="s">
-        <v>4</v>
+        <v>280</v>
       </c>
       <c r="M5" s="17"/>
       <c r="N5" s="14"/>
@@ -2234,20 +2237,20 @@
       <c r="F7" s="25"/>
       <c r="G7" s="24"/>
       <c r="H7" s="24"/>
-      <c r="I7" s="86" t="s">
+      <c r="I7" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="86"/>
+      <c r="J7" s="87"/>
       <c r="K7" s="26"/>
       <c r="L7" s="24"/>
       <c r="M7" s="27"/>
       <c r="N7" s="24"/>
       <c r="O7" s="24"/>
-      <c r="P7" s="86" t="s">
+      <c r="P7" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="Q7" s="86"/>
-      <c r="R7" s="86"/>
+      <c r="Q7" s="87"/>
+      <c r="R7" s="87"/>
       <c r="S7" s="24"/>
     </row>
     <row r="8" spans="1:19" ht="32.85" customHeight="1" x14ac:dyDescent="0.25">
@@ -2294,7 +2297,7 @@
         <v>21</v>
       </c>
       <c r="O8" s="29" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="P8" s="29" t="s">
         <v>22</v>
@@ -2321,10 +2324,10 @@
         <v>11111</v>
       </c>
       <c r="G9" s="67" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H9" s="67" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I9" s="68" t="s">
         <v>28</v>
@@ -2355,7 +2358,7 @@
         <v>223</v>
       </c>
       <c r="S9" s="73" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2370,19 +2373,19 @@
         <v>22222</v>
       </c>
       <c r="G10" s="67" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H10" s="67" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I10" s="68" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J10" s="74"/>
       <c r="K10" s="75"/>
       <c r="L10" s="67"/>
       <c r="M10" s="69" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="N10" s="70" t="s">
         <v>42</v>
@@ -2400,7 +2403,7 @@
         <v>224</v>
       </c>
       <c r="S10" s="73" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -2412,28 +2415,28 @@
       <c r="D11" s="34"/>
       <c r="E11" s="34"/>
       <c r="F11" s="76">
-        <v>33333</v>
+        <v>33334</v>
       </c>
       <c r="G11" s="67" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H11" s="67" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I11" s="77" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J11" s="78"/>
       <c r="K11" s="75"/>
       <c r="L11" s="79"/>
       <c r="M11" s="69" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="N11" s="70" t="s">
         <v>42</v>
       </c>
       <c r="O11" s="67" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="P11" s="71" t="s">
         <v>213</v>
@@ -2445,7 +2448,7 @@
         <v>224</v>
       </c>
       <c r="S11" s="73" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2457,16 +2460,16 @@
       <c r="D12" s="34"/>
       <c r="E12" s="34"/>
       <c r="F12" s="76">
-        <v>44444</v>
+        <v>44445</v>
       </c>
       <c r="G12" s="67" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H12" s="75" t="s">
         <v>38</v>
       </c>
       <c r="I12" s="77" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J12" s="78"/>
       <c r="K12" s="75" t="s">
@@ -2476,7 +2479,7 @@
         <v>100</v>
       </c>
       <c r="M12" s="69" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="N12" s="70" t="s">
         <v>220</v>
@@ -2493,8 +2496,8 @@
       <c r="R12" s="71" t="s">
         <v>223</v>
       </c>
-      <c r="S12" s="81" t="s">
-        <v>266</v>
+      <c r="S12" s="82" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2506,16 +2509,16 @@
       <c r="D13" s="34"/>
       <c r="E13" s="34"/>
       <c r="F13" s="76">
-        <v>44444</v>
+        <v>44445</v>
       </c>
       <c r="G13" s="67" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H13" s="75" t="s">
         <v>38</v>
       </c>
       <c r="I13" s="77" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J13" s="78"/>
       <c r="K13" s="75" t="s">
@@ -2525,7 +2528,7 @@
         <v>100</v>
       </c>
       <c r="M13" s="69" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="N13" s="70" t="s">
         <v>220</v>
@@ -2540,11 +2543,11 @@
         <v>6</v>
       </c>
       <c r="R13" s="71" t="s">
-        <v>252</v>
-      </c>
-      <c r="S13" s="82"/>
-    </row>
-    <row r="14" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+      <c r="S13" s="83"/>
+    </row>
+    <row r="14" spans="1:19" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33">
         <v>6</v>
       </c>
@@ -2553,16 +2556,16 @@
       <c r="D14" s="34"/>
       <c r="E14" s="34"/>
       <c r="F14" s="76">
-        <v>55555</v>
+        <v>55556</v>
       </c>
       <c r="G14" s="75" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H14" s="75" t="s">
         <v>38</v>
       </c>
       <c r="I14" s="77" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J14" s="78"/>
       <c r="K14" s="75" t="s">
@@ -2572,7 +2575,7 @@
         <v>47</v>
       </c>
       <c r="M14" s="69" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="N14" s="70" t="s">
         <v>220</v>
@@ -2589,11 +2592,9 @@
       <c r="R14" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="S14" s="73" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S14" s="81"/>
+    </row>
+    <row r="15" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="33">
         <v>7</v>
       </c>
@@ -2602,41 +2603,47 @@
       <c r="D15" s="34"/>
       <c r="E15" s="34"/>
       <c r="F15" s="76">
-        <v>66666</v>
-      </c>
-      <c r="G15" s="67" t="s">
-        <v>272</v>
+        <v>55556</v>
+      </c>
+      <c r="G15" s="75" t="s">
+        <v>256</v>
       </c>
       <c r="H15" s="75" t="s">
         <v>38</v>
       </c>
       <c r="I15" s="77" t="s">
-        <v>273</v>
+        <v>260</v>
       </c>
       <c r="J15" s="78"/>
       <c r="K15" s="75" t="s">
-        <v>115</v>
+        <v>35</v>
       </c>
       <c r="L15" s="79">
-        <v>200</v>
+        <v>47</v>
       </c>
       <c r="M15" s="69" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="N15" s="70" t="s">
         <v>220</v>
       </c>
       <c r="O15" s="67" t="s">
-        <v>36</v>
-      </c>
-      <c r="P15" s="71"/>
-      <c r="Q15" s="72"/>
-      <c r="R15" s="71"/>
+        <v>32</v>
+      </c>
+      <c r="P15" s="71" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q15" s="72">
+        <v>3</v>
+      </c>
+      <c r="R15" s="71" t="s">
+        <v>10</v>
+      </c>
       <c r="S15" s="73" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="33">
         <v>8</v>
       </c>
@@ -2645,16 +2652,16 @@
       <c r="D16" s="34"/>
       <c r="E16" s="34"/>
       <c r="F16" s="76">
-        <v>77777</v>
+        <v>66667</v>
       </c>
       <c r="G16" s="67" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="H16" s="75" t="s">
         <v>38</v>
       </c>
       <c r="I16" s="77" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="J16" s="78"/>
       <c r="K16" s="75" t="s">
@@ -2664,22 +2671,22 @@
         <v>200</v>
       </c>
       <c r="M16" s="69" t="s">
-        <v>264</v>
+        <v>273</v>
       </c>
       <c r="N16" s="70" t="s">
-        <v>42</v>
+        <v>220</v>
       </c>
       <c r="O16" s="67" t="s">
-        <v>267</v>
+        <v>36</v>
       </c>
       <c r="P16" s="71"/>
       <c r="Q16" s="72"/>
       <c r="R16" s="71"/>
       <c r="S16" s="73" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="33">
         <v>9</v>
       </c>
@@ -2688,16 +2695,16 @@
       <c r="D17" s="34"/>
       <c r="E17" s="34"/>
       <c r="F17" s="76">
-        <v>7777</v>
+        <v>77777</v>
       </c>
       <c r="G17" s="67" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="H17" s="75" t="s">
         <v>38</v>
       </c>
       <c r="I17" s="77" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="J17" s="78"/>
       <c r="K17" s="75" t="s">
@@ -2707,16 +2714,20 @@
         <v>200</v>
       </c>
       <c r="M17" s="69" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="N17" s="70" t="s">
         <v>42</v>
       </c>
-      <c r="O17" s="67"/>
+      <c r="O17" s="67" t="s">
+        <v>36</v>
+      </c>
       <c r="P17" s="71"/>
       <c r="Q17" s="72"/>
       <c r="R17" s="71"/>
-      <c r="S17" s="73"/>
+      <c r="S17" s="73" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="18" spans="1:19" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="33">
@@ -2727,40 +2738,34 @@
       <c r="D18" s="34"/>
       <c r="E18" s="34"/>
       <c r="F18" s="76">
-        <v>44444</v>
+        <v>77777</v>
       </c>
       <c r="G18" s="67" t="s">
-        <v>256</v>
+        <v>279</v>
       </c>
       <c r="H18" s="75" t="s">
         <v>38</v>
       </c>
       <c r="I18" s="77" t="s">
-        <v>260</v>
+        <v>276</v>
       </c>
       <c r="J18" s="78"/>
       <c r="K18" s="75" t="s">
-        <v>70</v>
+        <v>115</v>
       </c>
       <c r="L18" s="79">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="M18" s="69" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="N18" s="70" t="s">
-        <v>220</v>
-      </c>
-      <c r="O18" s="67" t="s">
-        <v>32</v>
-      </c>
-      <c r="P18" s="71" t="s">
-        <v>213</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="O18" s="67"/>
+      <c r="P18" s="71"/>
       <c r="Q18" s="72"/>
-      <c r="R18" s="71" t="s">
-        <v>252</v>
-      </c>
+      <c r="R18" s="71"/>
       <c r="S18" s="73"/>
     </row>
     <row r="19" spans="1:19" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2775,13 +2780,13 @@
         <v>44444</v>
       </c>
       <c r="G19" s="67" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H19" s="75" t="s">
         <v>38</v>
       </c>
       <c r="I19" s="77" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J19" s="78"/>
       <c r="K19" s="75" t="s">
@@ -2791,7 +2796,7 @@
         <v>100</v>
       </c>
       <c r="M19" s="69" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="N19" s="70" t="s">
         <v>220</v>
@@ -2799,12 +2804,12 @@
       <c r="O19" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="P19" s="71"/>
-      <c r="Q19" s="72">
-        <v>6</v>
-      </c>
+      <c r="P19" s="71" t="s">
+        <v>213</v>
+      </c>
+      <c r="Q19" s="72"/>
       <c r="R19" s="71" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="S19" s="73"/>
     </row>
@@ -2820,13 +2825,13 @@
         <v>44444</v>
       </c>
       <c r="G20" s="67" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H20" s="75" t="s">
         <v>38</v>
       </c>
       <c r="I20" s="77" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J20" s="78"/>
       <c r="K20" s="75" t="s">
@@ -2836,7 +2841,7 @@
         <v>100</v>
       </c>
       <c r="M20" s="69" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="N20" s="70" t="s">
         <v>220</v>
@@ -2844,12 +2849,12 @@
       <c r="O20" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="P20" s="71" t="s">
-        <v>202</v>
-      </c>
-      <c r="Q20" s="72"/>
+      <c r="P20" s="71"/>
+      <c r="Q20" s="72">
+        <v>6</v>
+      </c>
       <c r="R20" s="71" t="s">
-        <v>223</v>
+        <v>251</v>
       </c>
       <c r="S20" s="73"/>
     </row>
@@ -2865,13 +2870,13 @@
         <v>44444</v>
       </c>
       <c r="G21" s="67" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H21" s="75" t="s">
         <v>38</v>
       </c>
       <c r="I21" s="77" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J21" s="78"/>
       <c r="K21" s="75" t="s">
@@ -2881,7 +2886,7 @@
         <v>100</v>
       </c>
       <c r="M21" s="69" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="N21" s="70" t="s">
         <v>220</v>
@@ -2890,13 +2895,11 @@
         <v>32</v>
       </c>
       <c r="P21" s="71" t="s">
-        <v>213</v>
-      </c>
-      <c r="Q21" s="72">
-        <v>6</v>
-      </c>
+        <v>202</v>
+      </c>
+      <c r="Q21" s="72"/>
       <c r="R21" s="71" t="s">
-        <v>252</v>
+        <v>223</v>
       </c>
       <c r="S21" s="73"/>
     </row>
@@ -2908,25 +2911,47 @@
       <c r="C22" s="34"/>
       <c r="D22" s="34"/>
       <c r="E22" s="34"/>
-      <c r="F22" s="71"/>
-      <c r="G22" s="71"/>
-      <c r="H22" s="71"/>
-      <c r="I22" s="80"/>
-      <c r="J22" s="71"/>
-      <c r="K22" s="71"/>
-      <c r="L22" s="71"/>
-      <c r="M22" s="80"/>
-      <c r="N22" s="71"/>
-      <c r="O22" s="71"/>
-      <c r="P22" s="71"/>
-      <c r="Q22" s="72"/>
-      <c r="R22" s="71"/>
+      <c r="F22" s="76">
+        <v>44444</v>
+      </c>
+      <c r="G22" s="67" t="s">
+        <v>255</v>
+      </c>
+      <c r="H22" s="75" t="s">
+        <v>38</v>
+      </c>
+      <c r="I22" s="77" t="s">
+        <v>259</v>
+      </c>
+      <c r="J22" s="78"/>
+      <c r="K22" s="75" t="s">
+        <v>70</v>
+      </c>
+      <c r="L22" s="79">
+        <v>100</v>
+      </c>
+      <c r="M22" s="69" t="s">
+        <v>263</v>
+      </c>
+      <c r="N22" s="70" t="s">
+        <v>220</v>
+      </c>
+      <c r="O22" s="67" t="s">
+        <v>32</v>
+      </c>
+      <c r="P22" s="71" t="s">
+        <v>213</v>
+      </c>
+      <c r="Q22" s="72">
+        <v>6</v>
+      </c>
+      <c r="R22" s="71" t="s">
+        <v>251</v>
+      </c>
       <c r="S22" s="73"/>
     </row>
     <row r="23" spans="1:19" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="33">
-        <v>15</v>
-      </c>
+      <c r="A23" s="33"/>
       <c r="B23" s="34"/>
       <c r="C23" s="34"/>
       <c r="D23" s="34"/>
@@ -2947,9 +2972,7 @@
       <c r="S23" s="73"/>
     </row>
     <row r="24" spans="1:19" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="33">
-        <v>16</v>
-      </c>
+      <c r="A24" s="33"/>
       <c r="B24" s="34"/>
       <c r="C24" s="34"/>
       <c r="D24" s="34"/>
@@ -2971,7 +2994,7 @@
     </row>
     <row r="25" spans="1:19" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="33">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B25" s="34"/>
       <c r="C25" s="34"/>
@@ -2994,7 +3017,7 @@
     </row>
     <row r="26" spans="1:19" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="33">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B26" s="34"/>
       <c r="C26" s="34"/>
@@ -3017,7 +3040,7 @@
     </row>
     <row r="27" spans="1:19" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="33">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="B27" s="34"/>
       <c r="C27" s="34"/>
@@ -3040,7 +3063,7 @@
     </row>
     <row r="28" spans="1:19" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="33">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="B28" s="34"/>
       <c r="C28" s="34"/>
@@ -3061,26 +3084,88 @@
       <c r="R28" s="71"/>
       <c r="S28" s="73"/>
     </row>
-    <row r="29" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:19" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="33">
+        <v>10</v>
+      </c>
+      <c r="B29" s="34"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="71"/>
+      <c r="G29" s="71"/>
+      <c r="H29" s="71"/>
+      <c r="I29" s="80"/>
+      <c r="J29" s="71"/>
+      <c r="K29" s="71"/>
+      <c r="L29" s="71"/>
+      <c r="M29" s="80"/>
+      <c r="N29" s="71"/>
+      <c r="O29" s="71"/>
+      <c r="P29" s="71"/>
+      <c r="Q29" s="72"/>
+      <c r="R29" s="71"/>
+      <c r="S29" s="73"/>
+    </row>
+    <row r="30" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="33">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="33">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="33">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="33">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="33">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="33">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="33">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="33">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="33">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="33">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="51" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3908,6 +3993,7 @@
     <row r="873" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="874" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="875" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="876" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="S12:S13"/>
@@ -3923,11 +4009,11 @@
       <formula1>43831</formula1>
       <formula2>51501</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Valor Inválido - Deve ser um número maior que 0,1" sqref="L11:L21" xr:uid="{F62D5BAE-C1FD-43D4-A918-81A18C9B42D8}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Valor Inválido - Deve ser um número maior que 0,1" sqref="L11:L22" xr:uid="{F62D5BAE-C1FD-43D4-A918-81A18C9B42D8}">
       <formula1>0.1</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Opção Inválida - Valor inválido" sqref="L9:L10 L22:L28" xr:uid="{51734D73-F39C-4937-BF49-DBCE348732EF}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Opção Inválida - Valor inválido" sqref="L9:L10 L23:L29" xr:uid="{51734D73-F39C-4937-BF49-DBCE348732EF}">
       <formula1>0.1</formula1>
       <formula2>10000</formula2>
     </dataValidation>
@@ -3935,7 +4021,7 @@
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="I9:I12 I13:I16" numberStoredAsText="1"/>
+    <ignoredError sqref="I15:I17 I9:I13" numberStoredAsText="1"/>
     <ignoredError sqref="M10" twoDigitTextYear="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>
@@ -3949,7 +4035,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>H9:H28</xm:sqref>
+          <xm:sqref>H9:H29</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{249D6B8B-8015-4626-AE5F-E0098080783B}">
           <x14:formula1>
@@ -3967,7 +4053,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>P9:P28</xm:sqref>
+          <xm:sqref>P9:P29</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="ORAL-Via Oral_x000a_SNE-Nasoentérica_x000a_SNG-Nasogástrica_x000a_SOG-Orogástrica_x000a_GGT-Gastrostomia_x000a_JEJ-Jejunostomia" xr:uid="{D11BD5FF-6240-46C2-803C-3CE639B8685D}">
           <x14:formula1>
@@ -3976,13 +4062,13 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>N9:N28</xm:sqref>
+          <xm:sqref>N9:N29</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Ad ↑-Adic acima_x000a_M-Manip na Dieta_x000a_MA-Manip em Água_x000a_S-Separado" xr:uid="{645DFCD9-CA1C-47EB-A6D9-2A17C49AD15A}">
           <x14:formula1>
             <xm:f>'Apresentação Modulo'!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>R9:R28</xm:sqref>
+          <xm:sqref>R9:R29</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Opção Inválida - Escolha uma embalagem entre as opções mostradas" xr:uid="{90BBA368-B4C9-42E3-B7CD-0C1080ECC6E6}">
           <x14:formula1>
@@ -3991,7 +4077,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>O9:O28</xm:sqref>
+          <xm:sqref>O9:O29</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Opção Inválida - A dieta deve estar dentro das opções mostradas na lista" xr:uid="{DBFF39C0-9F9C-4C83-A4B1-42859471925A}">
           <x14:formula1>
@@ -4000,7 +4086,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>K9:K28</xm:sqref>
+          <xm:sqref>K9:K29</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Entre SIM se paciente mudou de leito desde a última prescrição. Entre NÃO, ou deixe em branco, caso contrário." xr:uid="{8A4458E0-478F-437B-9354-7FC5CE8E73D2}">
           <x14:formula1>
@@ -4009,7 +4095,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>J9:J28</xm:sqref>
+          <xm:sqref>J9:J29</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4034,10 +4120,10 @@
   <sheetData>
     <row r="1" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="61" t="s">
+        <v>231</v>
+      </c>
+      <c r="D1" s="59" t="s">
         <v>232</v>
-      </c>
-      <c r="D1" s="59" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4047,62 +4133,62 @@
     </row>
     <row r="3" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4112,12 +4198,12 @@
     </row>
     <row r="16" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -4141,17 +4227,17 @@
   <sheetData>
     <row r="1" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="61" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="62" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="62" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -4196,68 +4282,68 @@
   <sheetData>
     <row r="1" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="84" t="s">
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
-      <c r="K1" s="84"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="85" t="s">
-        <v>270</v>
-      </c>
-      <c r="N1" s="85"/>
-      <c r="O1" s="85"/>
-      <c r="P1" s="85"/>
-      <c r="Q1" s="85"/>
-      <c r="R1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
+      <c r="L1" s="85"/>
+      <c r="M1" s="86" t="s">
+        <v>269</v>
+      </c>
+      <c r="N1" s="86"/>
+      <c r="O1" s="86"/>
+      <c r="P1" s="86"/>
+      <c r="Q1" s="86"/>
+      <c r="R1" s="86"/>
     </row>
     <row r="2" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="85"/>
-      <c r="N2" s="85"/>
-      <c r="O2" s="85"/>
-      <c r="P2" s="85"/>
-      <c r="Q2" s="85"/>
-      <c r="R2" s="85"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="86"/>
+      <c r="O2" s="86"/>
+      <c r="P2" s="86"/>
+      <c r="Q2" s="86"/>
+      <c r="R2" s="86"/>
       <c r="S2" s="4"/>
     </row>
     <row r="3" spans="1:19" ht="3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
-      <c r="B3" s="83"/>
-      <c r="C3" s="83"/>
-      <c r="D3" s="83"/>
-      <c r="E3" s="83"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="84"/>
-      <c r="H3" s="84"/>
-      <c r="I3" s="84"/>
-      <c r="J3" s="84"/>
-      <c r="K3" s="84"/>
-      <c r="L3" s="84"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="85"/>
-      <c r="O3" s="85"/>
-      <c r="P3" s="85"/>
-      <c r="Q3" s="85"/>
-      <c r="R3" s="85"/>
+      <c r="B3" s="84"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="86"/>
+      <c r="N3" s="86"/>
+      <c r="O3" s="86"/>
+      <c r="P3" s="86"/>
+      <c r="Q3" s="86"/>
+      <c r="R3" s="86"/>
       <c r="S3" s="4"/>
     </row>
     <row r="4" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4326,20 +4412,20 @@
       <c r="F7" s="25"/>
       <c r="G7" s="24"/>
       <c r="H7" s="24"/>
-      <c r="I7" s="86" t="s">
+      <c r="I7" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="86"/>
+      <c r="J7" s="87"/>
       <c r="K7" s="26"/>
       <c r="L7" s="24"/>
       <c r="M7" s="27"/>
       <c r="N7" s="24"/>
       <c r="O7" s="24"/>
-      <c r="P7" s="86" t="s">
+      <c r="P7" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="Q7" s="86"/>
-      <c r="R7" s="86"/>
+      <c r="Q7" s="87"/>
+      <c r="R7" s="87"/>
       <c r="S7" s="24"/>
     </row>
     <row r="8" spans="1:19" ht="32.85" customHeight="1" x14ac:dyDescent="0.25">
@@ -4386,7 +4472,7 @@
         <v>21</v>
       </c>
       <c r="O8" s="29" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="P8" s="29" t="s">
         <v>22</v>
@@ -7323,117 +7409,117 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="87"/>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="88" t="s">
+      <c r="A1" s="95"/>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="96" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="88"/>
-      <c r="G1" s="88"/>
-      <c r="H1" s="88"/>
-      <c r="I1" s="88"/>
-      <c r="J1" s="89" t="s">
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
+      <c r="J1" s="97" t="s">
         <v>51</v>
       </c>
-      <c r="K1" s="89"/>
-      <c r="L1" s="89"/>
-      <c r="M1" s="89"/>
+      <c r="K1" s="97"/>
+      <c r="L1" s="97"/>
+      <c r="M1" s="97"/>
     </row>
     <row r="2" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="87"/>
-      <c r="B2" s="87"/>
-      <c r="C2" s="87"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
+      <c r="A2" s="95"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
     </row>
     <row r="3" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="87"/>
-      <c r="B3" s="87"/>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
-      <c r="H3" s="88"/>
-      <c r="I3" s="88"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
+      <c r="A3" s="95"/>
+      <c r="B3" s="95"/>
+      <c r="C3" s="95"/>
+      <c r="D3" s="95"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="97"/>
+      <c r="M3" s="97"/>
     </row>
     <row r="4" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="90" t="s">
+      <c r="A4" s="92" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="90"/>
-      <c r="C4" s="90"/>
-      <c r="D4" s="90"/>
-      <c r="E4" s="90" t="s">
+      <c r="B4" s="92"/>
+      <c r="C4" s="92"/>
+      <c r="D4" s="92"/>
+      <c r="E4" s="92" t="s">
         <v>53</v>
       </c>
-      <c r="F4" s="90"/>
+      <c r="F4" s="92"/>
       <c r="G4" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="H4" s="90" t="s">
+      <c r="H4" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="I4" s="90"/>
-      <c r="J4" s="90" t="s">
+      <c r="I4" s="92"/>
+      <c r="J4" s="92" t="s">
         <v>56</v>
       </c>
-      <c r="K4" s="90"/>
-      <c r="L4" s="90" t="s">
+      <c r="K4" s="92"/>
+      <c r="L4" s="92" t="s">
         <v>57</v>
       </c>
-      <c r="M4" s="90"/>
+      <c r="M4" s="92"/>
     </row>
     <row r="5" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="91">
+      <c r="A5" s="88">
         <v>1</v>
       </c>
-      <c r="B5" s="91"/>
-      <c r="C5" s="91"/>
-      <c r="D5" s="91"/>
-      <c r="E5" s="92" t="s">
+      <c r="B5" s="88"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="94" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="92"/>
+      <c r="F5" s="94"/>
       <c r="G5" s="55" t="s">
         <v>59</v>
       </c>
-      <c r="H5" s="91" t="s">
+      <c r="H5" s="88" t="s">
         <v>60</v>
       </c>
-      <c r="I5" s="91"/>
-      <c r="J5" s="91" t="s">
+      <c r="I5" s="88"/>
+      <c r="J5" s="88" t="s">
         <v>60</v>
       </c>
-      <c r="K5" s="91"/>
-      <c r="L5" s="91" t="s">
+      <c r="K5" s="88"/>
+      <c r="L5" s="88" t="s">
         <v>61</v>
       </c>
-      <c r="M5" s="91"/>
+      <c r="M5" s="88"/>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="93" t="s">
+      <c r="A6" s="91" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="93"/>
-      <c r="C6" s="93"/>
-      <c r="D6" s="93"/>
-      <c r="E6" s="93"/>
-      <c r="F6" s="93"/>
+      <c r="B6" s="91"/>
+      <c r="C6" s="91"/>
+      <c r="D6" s="91"/>
+      <c r="E6" s="91"/>
+      <c r="F6" s="91"/>
       <c r="G6" s="56"/>
       <c r="H6" s="57"/>
       <c r="I6" s="57"/>
@@ -7443,88 +7529,88 @@
       <c r="M6" s="57"/>
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="90" t="s">
+      <c r="A7" s="92" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="90"/>
-      <c r="C7" s="90"/>
-      <c r="D7" s="90" t="s">
+      <c r="B7" s="92"/>
+      <c r="C7" s="92"/>
+      <c r="D7" s="92" t="s">
         <v>63</v>
       </c>
-      <c r="E7" s="90"/>
-      <c r="F7" s="90"/>
-      <c r="G7" s="94" t="s">
+      <c r="E7" s="92"/>
+      <c r="F7" s="92"/>
+      <c r="G7" s="93" t="s">
         <v>64</v>
       </c>
-      <c r="H7" s="94"/>
-      <c r="I7" s="94"/>
-      <c r="J7" s="94"/>
-      <c r="K7" s="94"/>
-      <c r="L7" s="94"/>
-      <c r="M7" s="94"/>
+      <c r="H7" s="93"/>
+      <c r="I7" s="93"/>
+      <c r="J7" s="93"/>
+      <c r="K7" s="93"/>
+      <c r="L7" s="93"/>
+      <c r="M7" s="93"/>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="91">
+      <c r="A8" s="88">
         <v>0</v>
       </c>
-      <c r="B8" s="91"/>
-      <c r="C8" s="91"/>
-      <c r="D8" s="95">
+      <c r="B8" s="88"/>
+      <c r="C8" s="88"/>
+      <c r="D8" s="89">
         <v>43009</v>
       </c>
-      <c r="E8" s="95"/>
-      <c r="F8" s="95"/>
-      <c r="G8" s="96" t="s">
+      <c r="E8" s="89"/>
+      <c r="F8" s="89"/>
+      <c r="G8" s="90" t="s">
         <v>65</v>
       </c>
-      <c r="H8" s="96"/>
-      <c r="I8" s="96"/>
-      <c r="J8" s="96"/>
-      <c r="K8" s="96"/>
-      <c r="L8" s="96"/>
-      <c r="M8" s="96"/>
+      <c r="H8" s="90"/>
+      <c r="I8" s="90"/>
+      <c r="J8" s="90"/>
+      <c r="K8" s="90"/>
+      <c r="L8" s="90"/>
+      <c r="M8" s="90"/>
     </row>
     <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="91">
+      <c r="A9" s="88">
         <v>1</v>
       </c>
-      <c r="B9" s="91"/>
-      <c r="C9" s="91"/>
-      <c r="D9" s="95">
+      <c r="B9" s="88"/>
+      <c r="C9" s="88"/>
+      <c r="D9" s="89">
         <v>45238</v>
       </c>
-      <c r="E9" s="95"/>
-      <c r="F9" s="95"/>
-      <c r="G9" s="96" t="s">
+      <c r="E9" s="89"/>
+      <c r="F9" s="89"/>
+      <c r="G9" s="90" t="s">
         <v>66</v>
       </c>
-      <c r="H9" s="96"/>
-      <c r="I9" s="96"/>
-      <c r="J9" s="96"/>
-      <c r="K9" s="96"/>
-      <c r="L9" s="96"/>
-      <c r="M9" s="96"/>
+      <c r="H9" s="90"/>
+      <c r="I9" s="90"/>
+      <c r="J9" s="90"/>
+      <c r="K9" s="90"/>
+      <c r="L9" s="90"/>
+      <c r="M9" s="90"/>
     </row>
     <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="91">
+      <c r="A10" s="88">
         <v>2</v>
       </c>
-      <c r="B10" s="91"/>
-      <c r="C10" s="91"/>
-      <c r="D10" s="95">
+      <c r="B10" s="88"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="89">
         <v>45405</v>
       </c>
-      <c r="E10" s="95"/>
-      <c r="F10" s="95"/>
-      <c r="G10" s="96" t="s">
+      <c r="E10" s="89"/>
+      <c r="F10" s="89"/>
+      <c r="G10" s="90" t="s">
         <v>67</v>
       </c>
-      <c r="H10" s="96"/>
-      <c r="I10" s="96"/>
-      <c r="J10" s="96"/>
-      <c r="K10" s="96"/>
-      <c r="L10" s="96"/>
-      <c r="M10" s="96"/>
+      <c r="H10" s="90"/>
+      <c r="I10" s="90"/>
+      <c r="J10" s="90"/>
+      <c r="K10" s="90"/>
+      <c r="L10" s="90"/>
+      <c r="M10" s="90"/>
     </row>
     <row r="11" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8518,24 +8604,6 @@
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="G9:M9"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="G10:M10"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="G7:M7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="G8:M8"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="L5:M5"/>
     <mergeCell ref="A1:D3"/>
     <mergeCell ref="E1:I3"/>
     <mergeCell ref="J1:M3"/>
@@ -8544,6 +8612,24 @@
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="L4:M4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G7:M7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="G8:M8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="G9:M9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="G10:M10"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" fitToHeight="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -9439,7 +9525,7 @@
     </row>
     <row r="2" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -9510,7 +9596,7 @@
     </row>
     <row r="7" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -9529,7 +9615,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9551,7 +9637,7 @@
     </row>
     <row r="3" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="62" t="s">
-        <v>231</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Funcionando usando todas as linhas da df
</commit_message>
<xml_diff>
--- a/PLANILHA MÓDULOS V0.xlsx
+++ b/PLANILHA MÓDULOS V0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel Guido\Desktop\Github Repositories\PrimeiroBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBDA4343-FA26-4B26-AAC9-C80518C5184C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20FE6B73-6A8A-4A15-A71A-978E5F740271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="405" yWindow="360" windowWidth="20460" windowHeight="10770" tabRatio="982" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10140" yWindow="0" windowWidth="10455" windowHeight="10905" tabRatio="982" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exemplos Módulo" sheetId="11" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="270">
   <si>
     <t>DOCUMENTO RETIDO
 PLANILHA DE PEDIDOS PADRONIZADOS</t>
@@ -815,9 +815,6 @@
     <t>PACIENTE 04</t>
   </si>
   <si>
-    <t>PACIENTE 05</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
@@ -827,9 +824,6 @@
     <t>4</t>
   </si>
   <si>
-    <t>5</t>
-  </si>
-  <si>
     <t>3/6/9</t>
   </si>
   <si>
@@ -851,37 +845,10 @@
     <t>Paciente 03: 6 gr de Simbioflora enviado na embalagem original do produto (sachê nesse caso)</t>
   </si>
   <si>
-    <t>Paciente 05: 47ml de NAN Supreme 1, acrescido de 3 ml de TCM, totalizando 50ml de dieta, enviados na seringa</t>
-  </si>
-  <si>
     <t>Identificação: REG-POP-CPR-001-2</t>
   </si>
   <si>
     <t>Paciente 02: 11 gr de Espefor, somente o pó, pesado e enviado no coletor</t>
-  </si>
-  <si>
-    <t>PACIENTE 06</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>12/15</t>
-  </si>
-  <si>
-    <t>Paciente 06: 200 ml de suplemento Impact enviado em Frasco</t>
-  </si>
-  <si>
-    <t>PACIENTE 07</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>Paciente 07: 200 ml de suplemento Impact enviado na embalagem original do produto</t>
-  </si>
-  <si>
-    <t>PACIENTE 08</t>
   </si>
   <si>
     <t>14:30</t>
@@ -1172,7 +1139,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1420,9 +1387,6 @@
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2092,10 +2056,10 @@
   </sheetPr>
   <dimension ref="A1:S877"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="P13" sqref="P13"/>
+      <selection pane="bottomLeft" activeCell="I18" sqref="A18:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2121,68 +2085,68 @@
   <sheetData>
     <row r="1" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="86" t="s">
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="86"/>
-      <c r="J1" s="86"/>
-      <c r="K1" s="86"/>
-      <c r="L1" s="86"/>
-      <c r="M1" s="87" t="s">
-        <v>269</v>
-      </c>
-      <c r="N1" s="87"/>
-      <c r="O1" s="87"/>
-      <c r="P1" s="87"/>
-      <c r="Q1" s="87"/>
-      <c r="R1" s="87"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
+      <c r="L1" s="85"/>
+      <c r="M1" s="86" t="s">
+        <v>266</v>
+      </c>
+      <c r="N1" s="86"/>
+      <c r="O1" s="86"/>
+      <c r="P1" s="86"/>
+      <c r="Q1" s="86"/>
+      <c r="R1" s="86"/>
     </row>
     <row r="2" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="87"/>
-      <c r="N2" s="87"/>
-      <c r="O2" s="87"/>
-      <c r="P2" s="87"/>
-      <c r="Q2" s="87"/>
-      <c r="R2" s="87"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="86"/>
+      <c r="O2" s="86"/>
+      <c r="P2" s="86"/>
+      <c r="Q2" s="86"/>
+      <c r="R2" s="86"/>
       <c r="S2" s="4"/>
     </row>
     <row r="3" spans="1:19" ht="3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
-      <c r="B3" s="85"/>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="86"/>
-      <c r="J3" s="86"/>
-      <c r="K3" s="86"/>
-      <c r="L3" s="86"/>
-      <c r="M3" s="87"/>
-      <c r="N3" s="87"/>
-      <c r="O3" s="87"/>
-      <c r="P3" s="87"/>
-      <c r="Q3" s="87"/>
-      <c r="R3" s="87"/>
+      <c r="B3" s="84"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="86"/>
+      <c r="N3" s="86"/>
+      <c r="O3" s="86"/>
+      <c r="P3" s="86"/>
+      <c r="Q3" s="86"/>
+      <c r="R3" s="86"/>
       <c r="S3" s="4"/>
     </row>
     <row r="4" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2213,7 +2177,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="H5" s="15"/>
       <c r="I5" s="13"/>
@@ -2222,7 +2186,7 @@
         <v>3</v>
       </c>
       <c r="L5" s="64" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="M5" s="17"/>
       <c r="N5" s="14"/>
@@ -2251,20 +2215,20 @@
       <c r="F7" s="25"/>
       <c r="G7" s="24"/>
       <c r="H7" s="24"/>
-      <c r="I7" s="88" t="s">
+      <c r="I7" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="88"/>
+      <c r="J7" s="87"/>
       <c r="K7" s="26"/>
       <c r="L7" s="24"/>
       <c r="M7" s="27"/>
       <c r="N7" s="24"/>
       <c r="O7" s="24"/>
-      <c r="P7" s="88" t="s">
+      <c r="P7" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="Q7" s="88"/>
-      <c r="R7" s="88"/>
+      <c r="Q7" s="87"/>
+      <c r="R7" s="87"/>
       <c r="S7" s="24"/>
     </row>
     <row r="8" spans="1:19" ht="32.85" customHeight="1" x14ac:dyDescent="0.25">
@@ -2372,7 +2336,7 @@
         <v>223</v>
       </c>
       <c r="S9" s="73" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2393,13 +2357,13 @@
         <v>243</v>
       </c>
       <c r="I10" s="68" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J10" s="74"/>
       <c r="K10" s="75"/>
       <c r="L10" s="67"/>
       <c r="M10" s="69" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="N10" s="70" t="s">
         <v>42</v>
@@ -2417,7 +2381,7 @@
         <v>224</v>
       </c>
       <c r="S10" s="73" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -2438,19 +2402,19 @@
         <v>243</v>
       </c>
       <c r="I11" s="77" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J11" s="78"/>
       <c r="K11" s="75"/>
       <c r="L11" s="79"/>
       <c r="M11" s="69" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="N11" s="70" t="s">
         <v>42</v>
       </c>
       <c r="O11" s="67" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="P11" s="71" t="s">
         <v>213</v>
@@ -2462,47 +2426,47 @@
         <v>224</v>
       </c>
       <c r="S11" s="73" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="33">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B12" s="34"/>
       <c r="C12" s="34"/>
       <c r="D12" s="34"/>
       <c r="E12" s="34"/>
-      <c r="F12" s="76">
-        <v>44445</v>
+      <c r="F12" s="66">
+        <v>11111</v>
       </c>
       <c r="G12" s="67" t="s">
-        <v>255</v>
-      </c>
-      <c r="H12" s="75" t="s">
-        <v>38</v>
-      </c>
-      <c r="I12" s="77" t="s">
-        <v>259</v>
-      </c>
-      <c r="J12" s="78"/>
-      <c r="K12" s="75" t="s">
+        <v>252</v>
+      </c>
+      <c r="H12" s="67" t="s">
+        <v>243</v>
+      </c>
+      <c r="I12" s="68" t="s">
+        <v>28</v>
+      </c>
+      <c r="J12" s="67"/>
+      <c r="K12" s="67" t="s">
         <v>70</v>
       </c>
-      <c r="L12" s="79">
-        <v>100</v>
+      <c r="L12" s="67">
+        <v>50</v>
       </c>
       <c r="M12" s="69" t="s">
-        <v>263</v>
+        <v>30</v>
       </c>
       <c r="N12" s="70" t="s">
         <v>220</v>
       </c>
       <c r="O12" s="67" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="P12" s="71" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="Q12" s="72">
         <v>10</v>
@@ -2510,92 +2474,86 @@
       <c r="R12" s="71" t="s">
         <v>223</v>
       </c>
-      <c r="S12" s="82" t="s">
-        <v>265</v>
+      <c r="S12" s="73" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="33">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B13" s="34"/>
       <c r="C13" s="34"/>
       <c r="D13" s="34"/>
       <c r="E13" s="34"/>
-      <c r="F13" s="76">
-        <v>44445</v>
+      <c r="F13" s="66">
+        <v>22222</v>
       </c>
       <c r="G13" s="67" t="s">
-        <v>255</v>
-      </c>
-      <c r="H13" s="75" t="s">
-        <v>38</v>
-      </c>
-      <c r="I13" s="77" t="s">
+        <v>253</v>
+      </c>
+      <c r="H13" s="67" t="s">
+        <v>243</v>
+      </c>
+      <c r="I13" s="68" t="s">
+        <v>256</v>
+      </c>
+      <c r="J13" s="74"/>
+      <c r="K13" s="75"/>
+      <c r="L13" s="67"/>
+      <c r="M13" s="69" t="s">
         <v>259</v>
       </c>
-      <c r="J13" s="78"/>
-      <c r="K13" s="75" t="s">
-        <v>70</v>
-      </c>
-      <c r="L13" s="79">
-        <v>100</v>
-      </c>
-      <c r="M13" s="69" t="s">
-        <v>263</v>
-      </c>
       <c r="N13" s="70" t="s">
-        <v>220</v>
+        <v>42</v>
       </c>
       <c r="O13" s="67" t="s">
-        <v>32</v>
+        <v>226</v>
       </c>
       <c r="P13" s="71" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="Q13" s="72">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="R13" s="71" t="s">
-        <v>251</v>
-      </c>
-      <c r="S13" s="83"/>
-    </row>
-    <row r="14" spans="1:19" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+      <c r="S13" s="73" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B14" s="34"/>
       <c r="C14" s="34"/>
       <c r="D14" s="34"/>
       <c r="E14" s="34"/>
       <c r="F14" s="76">
-        <v>44445</v>
+        <v>33333</v>
       </c>
       <c r="G14" s="67" t="s">
-        <v>255</v>
-      </c>
-      <c r="H14" s="75" t="s">
-        <v>38</v>
+        <v>254</v>
+      </c>
+      <c r="H14" s="67" t="s">
+        <v>243</v>
       </c>
       <c r="I14" s="77" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="J14" s="78"/>
-      <c r="K14" s="75" t="s">
-        <v>70</v>
-      </c>
-      <c r="L14" s="79">
-        <v>100</v>
-      </c>
+      <c r="K14" s="75"/>
+      <c r="L14" s="79"/>
       <c r="M14" s="69" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="N14" s="70" t="s">
-        <v>220</v>
+        <v>42</v>
       </c>
       <c r="O14" s="67" t="s">
-        <v>32</v>
+        <v>264</v>
       </c>
       <c r="P14" s="71" t="s">
         <v>213</v>
@@ -2604,39 +2562,41 @@
         <v>6</v>
       </c>
       <c r="R14" s="71" t="s">
-        <v>251</v>
-      </c>
-      <c r="S14" s="84"/>
+        <v>224</v>
+      </c>
+      <c r="S14" s="73" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="15" spans="1:19" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="33">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B15" s="34"/>
       <c r="C15" s="34"/>
       <c r="D15" s="34"/>
       <c r="E15" s="34"/>
       <c r="F15" s="76">
-        <v>55556</v>
-      </c>
-      <c r="G15" s="75" t="s">
-        <v>256</v>
+        <v>44444</v>
+      </c>
+      <c r="G15" s="67" t="s">
+        <v>255</v>
       </c>
       <c r="H15" s="75" t="s">
         <v>38</v>
       </c>
       <c r="I15" s="77" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="J15" s="78"/>
       <c r="K15" s="75" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="L15" s="79">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="M15" s="69" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="N15" s="70" t="s">
         <v>220</v>
@@ -2645,45 +2605,47 @@
         <v>32</v>
       </c>
       <c r="P15" s="71" t="s">
-        <v>215</v>
+        <v>195</v>
       </c>
       <c r="Q15" s="72">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="R15" s="71" t="s">
-        <v>10</v>
-      </c>
-      <c r="S15" s="81"/>
-    </row>
-    <row r="16" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+      <c r="S15" s="81" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="33">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B16" s="34"/>
       <c r="C16" s="34"/>
       <c r="D16" s="34"/>
       <c r="E16" s="34"/>
       <c r="F16" s="76">
-        <v>55556</v>
-      </c>
-      <c r="G16" s="75" t="s">
-        <v>256</v>
+        <v>44444</v>
+      </c>
+      <c r="G16" s="67" t="s">
+        <v>255</v>
       </c>
       <c r="H16" s="75" t="s">
         <v>38</v>
       </c>
       <c r="I16" s="77" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="J16" s="78"/>
       <c r="K16" s="75" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="L16" s="79">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="M16" s="69" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="N16" s="70" t="s">
         <v>220</v>
@@ -2695,320 +2657,184 @@
         <v>215</v>
       </c>
       <c r="Q16" s="72">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="R16" s="71" t="s">
-        <v>10</v>
-      </c>
-      <c r="S16" s="73" t="s">
-        <v>268</v>
-      </c>
+        <v>251</v>
+      </c>
+      <c r="S16" s="82"/>
     </row>
     <row r="17" spans="1:19" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="33">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B17" s="34"/>
       <c r="C17" s="34"/>
       <c r="D17" s="34"/>
       <c r="E17" s="34"/>
       <c r="F17" s="76">
-        <v>66667</v>
+        <v>44444</v>
       </c>
       <c r="G17" s="67" t="s">
-        <v>271</v>
+        <v>255</v>
       </c>
       <c r="H17" s="75" t="s">
         <v>38</v>
       </c>
       <c r="I17" s="77" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="J17" s="78"/>
       <c r="K17" s="75" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="L17" s="79">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="M17" s="69" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="N17" s="70" t="s">
         <v>220</v>
       </c>
       <c r="O17" s="67" t="s">
-        <v>36</v>
-      </c>
-      <c r="P17" s="71"/>
-      <c r="Q17" s="72"/>
-      <c r="R17" s="71"/>
-      <c r="S17" s="73" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="33">
-        <v>9</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="P17" s="71" t="s">
+        <v>213</v>
+      </c>
+      <c r="Q17" s="72">
+        <v>6</v>
+      </c>
+      <c r="R17" s="71" t="s">
+        <v>251</v>
+      </c>
+      <c r="S17" s="83"/>
+    </row>
+    <row r="18" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="33"/>
       <c r="B18" s="34"/>
       <c r="C18" s="34"/>
       <c r="D18" s="34"/>
       <c r="E18" s="34"/>
-      <c r="F18" s="76">
-        <v>77777</v>
-      </c>
-      <c r="G18" s="67" t="s">
-        <v>275</v>
-      </c>
-      <c r="H18" s="75" t="s">
-        <v>38</v>
-      </c>
-      <c r="I18" s="77" t="s">
-        <v>276</v>
-      </c>
+      <c r="F18" s="76"/>
+      <c r="G18" s="75"/>
+      <c r="H18" s="75"/>
+      <c r="I18" s="77"/>
       <c r="J18" s="78"/>
-      <c r="K18" s="75" t="s">
-        <v>35</v>
-      </c>
-      <c r="L18" s="79">
-        <v>200</v>
-      </c>
-      <c r="M18" s="69" t="s">
-        <v>263</v>
-      </c>
-      <c r="N18" s="70" t="s">
-        <v>42</v>
-      </c>
-      <c r="O18" s="67" t="s">
-        <v>36</v>
-      </c>
+      <c r="K18" s="75"/>
+      <c r="L18" s="79"/>
+      <c r="M18" s="69"/>
+      <c r="N18" s="70"/>
+      <c r="O18" s="67"/>
       <c r="P18" s="71"/>
       <c r="Q18" s="72"/>
       <c r="R18" s="71"/>
-      <c r="S18" s="73" t="s">
-        <v>277</v>
-      </c>
+      <c r="S18" s="73"/>
     </row>
     <row r="19" spans="1:19" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="33">
-        <v>10</v>
-      </c>
+      <c r="A19" s="33"/>
       <c r="B19" s="34"/>
       <c r="C19" s="34"/>
       <c r="D19" s="34"/>
       <c r="E19" s="34"/>
-      <c r="F19" s="76">
-        <v>77777</v>
-      </c>
-      <c r="G19" s="67" t="s">
-        <v>278</v>
-      </c>
-      <c r="H19" s="75" t="s">
-        <v>38</v>
-      </c>
-      <c r="I19" s="77" t="s">
-        <v>276</v>
-      </c>
+      <c r="F19" s="76"/>
+      <c r="G19" s="67"/>
+      <c r="H19" s="75"/>
+      <c r="I19" s="77"/>
       <c r="J19" s="78"/>
-      <c r="K19" s="75" t="s">
-        <v>35</v>
-      </c>
-      <c r="L19" s="79">
-        <v>200</v>
-      </c>
-      <c r="M19" s="69" t="s">
-        <v>263</v>
-      </c>
-      <c r="N19" s="70" t="s">
-        <v>42</v>
-      </c>
+      <c r="K19" s="75"/>
+      <c r="L19" s="79"/>
+      <c r="M19" s="69"/>
+      <c r="N19" s="70"/>
       <c r="O19" s="67"/>
       <c r="P19" s="71"/>
       <c r="Q19" s="72"/>
       <c r="R19" s="71"/>
       <c r="S19" s="73"/>
     </row>
-    <row r="20" spans="1:19" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="33">
-        <v>11</v>
-      </c>
+    <row r="20" spans="1:19" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="33"/>
       <c r="B20" s="34"/>
       <c r="C20" s="34"/>
       <c r="D20" s="34"/>
       <c r="E20" s="34"/>
-      <c r="F20" s="76">
-        <v>44444</v>
-      </c>
-      <c r="G20" s="67" t="s">
-        <v>255</v>
-      </c>
-      <c r="H20" s="75" t="s">
-        <v>38</v>
-      </c>
-      <c r="I20" s="77" t="s">
-        <v>259</v>
-      </c>
+      <c r="F20" s="76"/>
+      <c r="G20" s="67"/>
+      <c r="H20" s="75"/>
+      <c r="I20" s="77"/>
       <c r="J20" s="78"/>
-      <c r="K20" s="75" t="s">
-        <v>70</v>
-      </c>
-      <c r="L20" s="79">
-        <v>100</v>
-      </c>
-      <c r="M20" s="69" t="s">
-        <v>263</v>
-      </c>
-      <c r="N20" s="70" t="s">
-        <v>220</v>
-      </c>
-      <c r="O20" s="67" t="s">
-        <v>32</v>
-      </c>
-      <c r="P20" s="71" t="s">
-        <v>213</v>
-      </c>
+      <c r="K20" s="75"/>
+      <c r="L20" s="79"/>
+      <c r="M20" s="69"/>
+      <c r="N20" s="70"/>
+      <c r="O20" s="67"/>
+      <c r="P20" s="71"/>
       <c r="Q20" s="72"/>
-      <c r="R20" s="71" t="s">
-        <v>251</v>
-      </c>
+      <c r="R20" s="71"/>
       <c r="S20" s="73"/>
     </row>
     <row r="21" spans="1:19" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="33">
-        <v>12</v>
-      </c>
+      <c r="A21" s="33"/>
       <c r="B21" s="34"/>
       <c r="C21" s="34"/>
       <c r="D21" s="34"/>
       <c r="E21" s="34"/>
-      <c r="F21" s="76">
-        <v>44444</v>
-      </c>
-      <c r="G21" s="67" t="s">
-        <v>255</v>
-      </c>
-      <c r="H21" s="75" t="s">
-        <v>38</v>
-      </c>
-      <c r="I21" s="77" t="s">
-        <v>259</v>
-      </c>
+      <c r="F21" s="76"/>
+      <c r="G21" s="67"/>
+      <c r="H21" s="75"/>
+      <c r="I21" s="77"/>
       <c r="J21" s="78"/>
-      <c r="K21" s="75" t="s">
-        <v>70</v>
-      </c>
-      <c r="L21" s="79">
-        <v>100</v>
-      </c>
-      <c r="M21" s="69" t="s">
-        <v>263</v>
-      </c>
-      <c r="N21" s="70" t="s">
-        <v>220</v>
-      </c>
-      <c r="O21" s="67" t="s">
-        <v>32</v>
-      </c>
+      <c r="K21" s="75"/>
+      <c r="L21" s="79"/>
+      <c r="M21" s="69"/>
+      <c r="N21" s="70"/>
+      <c r="O21" s="67"/>
       <c r="P21" s="71"/>
-      <c r="Q21" s="72">
-        <v>6</v>
-      </c>
-      <c r="R21" s="71" t="s">
-        <v>251</v>
-      </c>
+      <c r="Q21" s="72"/>
+      <c r="R21" s="71"/>
       <c r="S21" s="73"/>
     </row>
     <row r="22" spans="1:19" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="33">
-        <v>13</v>
-      </c>
+      <c r="A22" s="33"/>
       <c r="B22" s="34"/>
       <c r="C22" s="34"/>
       <c r="D22" s="34"/>
       <c r="E22" s="34"/>
-      <c r="F22" s="76">
-        <v>44444</v>
-      </c>
-      <c r="G22" s="67" t="s">
-        <v>255</v>
-      </c>
-      <c r="H22" s="75" t="s">
-        <v>38</v>
-      </c>
-      <c r="I22" s="77" t="s">
-        <v>259</v>
-      </c>
+      <c r="F22" s="76"/>
+      <c r="G22" s="67"/>
+      <c r="H22" s="75"/>
+      <c r="I22" s="77"/>
       <c r="J22" s="78"/>
-      <c r="K22" s="75" t="s">
-        <v>70</v>
-      </c>
-      <c r="L22" s="79">
-        <v>100</v>
-      </c>
-      <c r="M22" s="69" t="s">
-        <v>263</v>
-      </c>
-      <c r="N22" s="70" t="s">
-        <v>220</v>
-      </c>
-      <c r="O22" s="67" t="s">
-        <v>32</v>
-      </c>
-      <c r="P22" s="71" t="s">
-        <v>202</v>
-      </c>
+      <c r="K22" s="75"/>
+      <c r="L22" s="79"/>
+      <c r="M22" s="69"/>
+      <c r="N22" s="70"/>
+      <c r="O22" s="67"/>
+      <c r="P22" s="71"/>
       <c r="Q22" s="72"/>
-      <c r="R22" s="71" t="s">
-        <v>223</v>
-      </c>
+      <c r="R22" s="71"/>
       <c r="S22" s="73"/>
     </row>
     <row r="23" spans="1:19" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="33">
-        <v>14</v>
-      </c>
+      <c r="A23" s="33"/>
       <c r="B23" s="34"/>
       <c r="C23" s="34"/>
       <c r="D23" s="34"/>
       <c r="E23" s="34"/>
-      <c r="F23" s="76">
-        <v>44444</v>
-      </c>
-      <c r="G23" s="67" t="s">
-        <v>255</v>
-      </c>
-      <c r="H23" s="75" t="s">
-        <v>38</v>
-      </c>
-      <c r="I23" s="77" t="s">
-        <v>259</v>
-      </c>
+      <c r="F23" s="76"/>
+      <c r="G23" s="67"/>
+      <c r="H23" s="75"/>
+      <c r="I23" s="77"/>
       <c r="J23" s="78"/>
-      <c r="K23" s="75" t="s">
-        <v>70</v>
-      </c>
-      <c r="L23" s="79">
-        <v>100</v>
-      </c>
-      <c r="M23" s="69" t="s">
-        <v>263</v>
-      </c>
-      <c r="N23" s="70" t="s">
-        <v>220</v>
-      </c>
-      <c r="O23" s="67" t="s">
-        <v>32</v>
-      </c>
-      <c r="P23" s="71" t="s">
-        <v>213</v>
-      </c>
-      <c r="Q23" s="72">
-        <v>6</v>
-      </c>
-      <c r="R23" s="71" t="s">
-        <v>251</v>
-      </c>
+      <c r="K23" s="75"/>
+      <c r="L23" s="79"/>
+      <c r="M23" s="69"/>
+      <c r="N23" s="70"/>
+      <c r="O23" s="67"/>
+      <c r="P23" s="71"/>
+      <c r="Q23" s="72"/>
+      <c r="R23" s="71"/>
       <c r="S23" s="73"/>
     </row>
     <row r="24" spans="1:19" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4057,7 +3883,7 @@
     <row r="877" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="S12:S14"/>
+    <mergeCell ref="S15:S17"/>
     <mergeCell ref="B1:E3"/>
     <mergeCell ref="F1:L3"/>
     <mergeCell ref="M1:R3"/>
@@ -4070,11 +3896,11 @@
       <formula1>43831</formula1>
       <formula2>51501</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Valor Inválido - Deve ser um número maior que 0,1" sqref="L11:L23" xr:uid="{F62D5BAE-C1FD-43D4-A918-81A18C9B42D8}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Valor Inválido - Deve ser um número maior que 0,1" sqref="L11 L14:L23" xr:uid="{F62D5BAE-C1FD-43D4-A918-81A18C9B42D8}">
       <formula1>0.1</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Opção Inválida - Valor inválido" sqref="L9:L10 L24:L30" xr:uid="{51734D73-F39C-4937-BF49-DBCE348732EF}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Opção Inválida - Valor inválido" sqref="L9:L10 L24:L30 L12:L13" xr:uid="{51734D73-F39C-4937-BF49-DBCE348732EF}">
       <formula1>0.1</formula1>
       <formula2>10000</formula2>
     </dataValidation>
@@ -4082,7 +3908,7 @@
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="I16:I18 I14 I9:I12" numberStoredAsText="1"/>
+    <ignoredError sqref="I9:I11" numberStoredAsText="1"/>
     <ignoredError sqref="M10" twoDigitTextYear="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>
@@ -4096,7 +3922,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>H9:H30</xm:sqref>
+          <xm:sqref>H9:H11 H21:H30</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{249D6B8B-8015-4626-AE5F-E0098080783B}">
           <x14:formula1>
@@ -4114,7 +3940,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>P9:P30</xm:sqref>
+          <xm:sqref>P9:P11 P21:P30</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="ORAL-Via Oral_x000a_SNE-Nasoentérica_x000a_SNG-Nasogástrica_x000a_SOG-Orogástrica_x000a_GGT-Gastrostomia_x000a_JEJ-Jejunostomia" xr:uid="{D11BD5FF-6240-46C2-803C-3CE639B8685D}">
           <x14:formula1>
@@ -4123,13 +3949,13 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>N9:N30</xm:sqref>
+          <xm:sqref>N9:N11 N21:N30</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Ad ↑-Adic acima_x000a_M-Manip na Dieta_x000a_MA-Manip em Água_x000a_S-Separado" xr:uid="{645DFCD9-CA1C-47EB-A6D9-2A17C49AD15A}">
           <x14:formula1>
             <xm:f>'Apresentação Modulo'!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>R9:R30</xm:sqref>
+          <xm:sqref>R9:R11 R21:R30</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Opção Inválida - Escolha uma embalagem entre as opções mostradas" xr:uid="{90BBA368-B4C9-42E3-B7CD-0C1080ECC6E6}">
           <x14:formula1>
@@ -4138,7 +3964,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>O9:O30</xm:sqref>
+          <xm:sqref>O9:O11 O21:O30</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Opção Inválida - A dieta deve estar dentro das opções mostradas na lista" xr:uid="{DBFF39C0-9F9C-4C83-A4B1-42859471925A}">
           <x14:formula1>
@@ -4147,7 +3973,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>K9:K30</xm:sqref>
+          <xm:sqref>K9:K11 K21:K30</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Entre SIM se paciente mudou de leito desde a última prescrição. Entre NÃO, ou deixe em branco, caso contrário." xr:uid="{8A4458E0-478F-437B-9354-7FC5CE8E73D2}">
           <x14:formula1>
@@ -4156,7 +3982,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>J9:J30</xm:sqref>
+          <xm:sqref>J9:J11 J21:J30</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4343,68 +4169,68 @@
   <sheetData>
     <row r="1" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="86" t="s">
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="86"/>
-      <c r="J1" s="86"/>
-      <c r="K1" s="86"/>
-      <c r="L1" s="86"/>
-      <c r="M1" s="87" t="s">
-        <v>269</v>
-      </c>
-      <c r="N1" s="87"/>
-      <c r="O1" s="87"/>
-      <c r="P1" s="87"/>
-      <c r="Q1" s="87"/>
-      <c r="R1" s="87"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
+      <c r="L1" s="85"/>
+      <c r="M1" s="86" t="s">
+        <v>266</v>
+      </c>
+      <c r="N1" s="86"/>
+      <c r="O1" s="86"/>
+      <c r="P1" s="86"/>
+      <c r="Q1" s="86"/>
+      <c r="R1" s="86"/>
     </row>
     <row r="2" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="87"/>
-      <c r="N2" s="87"/>
-      <c r="O2" s="87"/>
-      <c r="P2" s="87"/>
-      <c r="Q2" s="87"/>
-      <c r="R2" s="87"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="86"/>
+      <c r="O2" s="86"/>
+      <c r="P2" s="86"/>
+      <c r="Q2" s="86"/>
+      <c r="R2" s="86"/>
       <c r="S2" s="4"/>
     </row>
     <row r="3" spans="1:19" ht="3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
-      <c r="B3" s="85"/>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="86"/>
-      <c r="J3" s="86"/>
-      <c r="K3" s="86"/>
-      <c r="L3" s="86"/>
-      <c r="M3" s="87"/>
-      <c r="N3" s="87"/>
-      <c r="O3" s="87"/>
-      <c r="P3" s="87"/>
-      <c r="Q3" s="87"/>
-      <c r="R3" s="87"/>
+      <c r="B3" s="84"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="86"/>
+      <c r="N3" s="86"/>
+      <c r="O3" s="86"/>
+      <c r="P3" s="86"/>
+      <c r="Q3" s="86"/>
+      <c r="R3" s="86"/>
       <c r="S3" s="4"/>
     </row>
     <row r="4" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4473,20 +4299,20 @@
       <c r="F7" s="25"/>
       <c r="G7" s="24"/>
       <c r="H7" s="24"/>
-      <c r="I7" s="88" t="s">
+      <c r="I7" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="88"/>
+      <c r="J7" s="87"/>
       <c r="K7" s="26"/>
       <c r="L7" s="24"/>
       <c r="M7" s="27"/>
       <c r="N7" s="24"/>
       <c r="O7" s="24"/>
-      <c r="P7" s="88" t="s">
+      <c r="P7" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="Q7" s="88"/>
-      <c r="R7" s="88"/>
+      <c r="Q7" s="87"/>
+      <c r="R7" s="87"/>
       <c r="S7" s="24"/>
     </row>
     <row r="8" spans="1:19" ht="32.85" customHeight="1" x14ac:dyDescent="0.25">
@@ -7470,117 +7296,117 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="89"/>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="90" t="s">
+      <c r="A1" s="88"/>
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="89" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="90"/>
-      <c r="J1" s="91" t="s">
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
+      <c r="J1" s="90" t="s">
         <v>51</v>
       </c>
-      <c r="K1" s="91"/>
-      <c r="L1" s="91"/>
-      <c r="M1" s="91"/>
+      <c r="K1" s="90"/>
+      <c r="L1" s="90"/>
+      <c r="M1" s="90"/>
     </row>
     <row r="2" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="89"/>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="91"/>
-      <c r="K2" s="91"/>
-      <c r="L2" s="91"/>
-      <c r="M2" s="91"/>
+      <c r="A2" s="88"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="90"/>
     </row>
     <row r="3" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="89"/>
-      <c r="B3" s="89"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="91"/>
-      <c r="L3" s="91"/>
-      <c r="M3" s="91"/>
+      <c r="A3" s="88"/>
+      <c r="B3" s="88"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="90"/>
+      <c r="M3" s="90"/>
     </row>
     <row r="4" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="92" t="s">
+      <c r="A4" s="91" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="92"/>
-      <c r="C4" s="92"/>
-      <c r="D4" s="92"/>
-      <c r="E4" s="92" t="s">
+      <c r="B4" s="91"/>
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="91" t="s">
         <v>53</v>
       </c>
-      <c r="F4" s="92"/>
+      <c r="F4" s="91"/>
       <c r="G4" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="H4" s="92" t="s">
+      <c r="H4" s="91" t="s">
         <v>55</v>
       </c>
-      <c r="I4" s="92"/>
-      <c r="J4" s="92" t="s">
+      <c r="I4" s="91"/>
+      <c r="J4" s="91" t="s">
         <v>56</v>
       </c>
-      <c r="K4" s="92"/>
-      <c r="L4" s="92" t="s">
+      <c r="K4" s="91"/>
+      <c r="L4" s="91" t="s">
         <v>57</v>
       </c>
-      <c r="M4" s="92"/>
+      <c r="M4" s="91"/>
     </row>
     <row r="5" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="93">
+      <c r="A5" s="92">
         <v>1</v>
       </c>
-      <c r="B5" s="93"/>
-      <c r="C5" s="93"/>
-      <c r="D5" s="93"/>
-      <c r="E5" s="94" t="s">
+      <c r="B5" s="92"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="92"/>
+      <c r="E5" s="93" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="94"/>
+      <c r="F5" s="93"/>
       <c r="G5" s="55" t="s">
         <v>59</v>
       </c>
-      <c r="H5" s="93" t="s">
+      <c r="H5" s="92" t="s">
         <v>60</v>
       </c>
-      <c r="I5" s="93"/>
-      <c r="J5" s="93" t="s">
+      <c r="I5" s="92"/>
+      <c r="J5" s="92" t="s">
         <v>60</v>
       </c>
-      <c r="K5" s="93"/>
-      <c r="L5" s="93" t="s">
+      <c r="K5" s="92"/>
+      <c r="L5" s="92" t="s">
         <v>61</v>
       </c>
-      <c r="M5" s="93"/>
+      <c r="M5" s="92"/>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="95" t="s">
+      <c r="A6" s="94" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="95"/>
-      <c r="C6" s="95"/>
-      <c r="D6" s="95"/>
-      <c r="E6" s="95"/>
-      <c r="F6" s="95"/>
+      <c r="B6" s="94"/>
+      <c r="C6" s="94"/>
+      <c r="D6" s="94"/>
+      <c r="E6" s="94"/>
+      <c r="F6" s="94"/>
       <c r="G6" s="56"/>
       <c r="H6" s="57"/>
       <c r="I6" s="57"/>
@@ -7590,88 +7416,88 @@
       <c r="M6" s="57"/>
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="92" t="s">
+      <c r="A7" s="91" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="92"/>
-      <c r="C7" s="92"/>
-      <c r="D7" s="92" t="s">
+      <c r="B7" s="91"/>
+      <c r="C7" s="91"/>
+      <c r="D7" s="91" t="s">
         <v>63</v>
       </c>
-      <c r="E7" s="92"/>
-      <c r="F7" s="92"/>
-      <c r="G7" s="96" t="s">
+      <c r="E7" s="91"/>
+      <c r="F7" s="91"/>
+      <c r="G7" s="95" t="s">
         <v>64</v>
       </c>
-      <c r="H7" s="96"/>
-      <c r="I7" s="96"/>
-      <c r="J7" s="96"/>
-      <c r="K7" s="96"/>
-      <c r="L7" s="96"/>
-      <c r="M7" s="96"/>
+      <c r="H7" s="95"/>
+      <c r="I7" s="95"/>
+      <c r="J7" s="95"/>
+      <c r="K7" s="95"/>
+      <c r="L7" s="95"/>
+      <c r="M7" s="95"/>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="93">
+      <c r="A8" s="92">
         <v>0</v>
       </c>
-      <c r="B8" s="93"/>
-      <c r="C8" s="93"/>
-      <c r="D8" s="97">
+      <c r="B8" s="92"/>
+      <c r="C8" s="92"/>
+      <c r="D8" s="96">
         <v>43009</v>
       </c>
-      <c r="E8" s="97"/>
-      <c r="F8" s="97"/>
-      <c r="G8" s="98" t="s">
+      <c r="E8" s="96"/>
+      <c r="F8" s="96"/>
+      <c r="G8" s="97" t="s">
         <v>65</v>
       </c>
-      <c r="H8" s="98"/>
-      <c r="I8" s="98"/>
-      <c r="J8" s="98"/>
-      <c r="K8" s="98"/>
-      <c r="L8" s="98"/>
-      <c r="M8" s="98"/>
+      <c r="H8" s="97"/>
+      <c r="I8" s="97"/>
+      <c r="J8" s="97"/>
+      <c r="K8" s="97"/>
+      <c r="L8" s="97"/>
+      <c r="M8" s="97"/>
     </row>
     <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="93">
+      <c r="A9" s="92">
         <v>1</v>
       </c>
-      <c r="B9" s="93"/>
-      <c r="C9" s="93"/>
-      <c r="D9" s="97">
+      <c r="B9" s="92"/>
+      <c r="C9" s="92"/>
+      <c r="D9" s="96">
         <v>45238</v>
       </c>
-      <c r="E9" s="97"/>
-      <c r="F9" s="97"/>
-      <c r="G9" s="98" t="s">
+      <c r="E9" s="96"/>
+      <c r="F9" s="96"/>
+      <c r="G9" s="97" t="s">
         <v>66</v>
       </c>
-      <c r="H9" s="98"/>
-      <c r="I9" s="98"/>
-      <c r="J9" s="98"/>
-      <c r="K9" s="98"/>
-      <c r="L9" s="98"/>
-      <c r="M9" s="98"/>
+      <c r="H9" s="97"/>
+      <c r="I9" s="97"/>
+      <c r="J9" s="97"/>
+      <c r="K9" s="97"/>
+      <c r="L9" s="97"/>
+      <c r="M9" s="97"/>
     </row>
     <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="93">
+      <c r="A10" s="92">
         <v>2</v>
       </c>
-      <c r="B10" s="93"/>
-      <c r="C10" s="93"/>
-      <c r="D10" s="97">
+      <c r="B10" s="92"/>
+      <c r="C10" s="92"/>
+      <c r="D10" s="96">
         <v>45405</v>
       </c>
-      <c r="E10" s="97"/>
-      <c r="F10" s="97"/>
-      <c r="G10" s="98" t="s">
+      <c r="E10" s="96"/>
+      <c r="F10" s="96"/>
+      <c r="G10" s="97" t="s">
         <v>67</v>
       </c>
-      <c r="H10" s="98"/>
-      <c r="I10" s="98"/>
-      <c r="J10" s="98"/>
-      <c r="K10" s="98"/>
-      <c r="L10" s="98"/>
-      <c r="M10" s="98"/>
+      <c r="H10" s="97"/>
+      <c r="I10" s="97"/>
+      <c r="J10" s="97"/>
+      <c r="K10" s="97"/>
+      <c r="L10" s="97"/>
+      <c r="M10" s="97"/>
     </row>
     <row r="11" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9657,7 +9483,7 @@
     </row>
     <row r="7" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -9698,7 +9524,7 @@
     </row>
     <row r="3" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="62" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>

</xml_diff>